<commit_message>
Correct the KEGG coloring
Correct the errors in the KEGG coloring.
</commit_message>
<xml_diff>
--- a/nbis_meta/3_Annotation/DESeq2/SigPathway.xlsx
+++ b/nbis_meta/3_Annotation/DESeq2/SigPathway.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1Lund_Lectures\BINP37_project_15\BINP37-Git\BINP37_Project\nbis_meta_test\3_Annotation\DESeq2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1Lund_Lectures\BINP37_project_15\BINP37-Git\BINP37_Project\nbis_meta\3_Annotation\DESeq2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6CDF05-BA64-4986-860F-A276691783E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462C6139-2A35-4A9B-B1E0-D8BD0ED41008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2-components" sheetId="1" r:id="rId1"/>
@@ -1057,1090 +1057,1091 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>M00357</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methanogenesis, acetate =&gt; methane</t>
+  </si>
+  <si>
+    <t>M00356</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methanogenesis, methanol =&gt; methane</t>
+  </si>
+  <si>
+    <t>M00563</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methanogenesis, methylamine/dimethylamine/trimethylamine =&gt; methane</t>
+  </si>
+  <si>
+    <t>M00358</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coenzyme M biosynthesis</t>
+  </si>
+  <si>
+    <t>M00608</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-Oxocarboxylic acid chain extension, 2-oxoglutarate =&gt; 2-oxoadipate =&gt; 2-oxopimelate =&gt; 2-oxosuberate</t>
+  </si>
+  <si>
+    <t>M00174</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methane oxidation, methanotroph, methane =&gt; formaldehyde</t>
+  </si>
+  <si>
+    <t>M00346</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Formaldehyde assimilation, serine pathway</t>
+  </si>
+  <si>
+    <t>M00345</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Formaldehyde assimilation, ribulose monophosphate pathway</t>
+  </si>
+  <si>
+    <t>M00344</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Formaldehyde assimilation, xylulose monophosphate pathway</t>
+  </si>
+  <si>
+    <t>M00378</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F420 biosynthesis, archaea</t>
+  </si>
+  <si>
+    <t>M00935</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methanofuran biosynthesis</t>
+  </si>
+  <si>
+    <t>M00422</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acetyl-CoA pathway, CO2 =&gt; acetyl-CoA</t>
+  </si>
+  <si>
+    <t>M00020</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Serine biosynthesis, glycerate-3P =&gt; serine</t>
+  </si>
+  <si>
+    <t>M00129</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ascorbate biosynthesis, animals, glucose-1P =&gt; ascorbate</t>
+  </si>
+  <si>
+    <t>uidA, AKR1A1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00114</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ascorbate biosynthesis, plants, fructose-6P =&gt; ascorbate</t>
+  </si>
+  <si>
+    <t>GMPP, VTC4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comB, comC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comA, comB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aksA, aksD, aksE, aksF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cofH, cofG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mfnA, mfnD, mfnF, mfnE, mfnB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mfnD, mfnF, mfnE, mfnC, mfnB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00049</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adenine ribonucleotide biosynthesis, IMP =&gt; ADP,ATP</t>
+  </si>
+  <si>
+    <t>M00051</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>De novo pyrimidine biosynthesis, glutamine (+ PRPP) =&gt; UMP</t>
+  </si>
+  <si>
+    <t>M00127</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thiamine biosynthesis, prokaryotes, AIR (+ DXP/tyrosine) =&gt; TMP/TPP</t>
+  </si>
+  <si>
+    <t>M00896</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thiamine biosynthesis, archaea, AIR (+ NAD+) =&gt; TMP/TPP</t>
+  </si>
+  <si>
+    <t>M00125</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Riboflavin biosynthesis, plants and bacteria, GTP =&gt; riboflavin/FMN/FAD</t>
+  </si>
+  <si>
+    <t>ribD1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00911</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Riboflavin biosynthesis, fungi, GTP =&gt; riboflavin/FMN/FAD</t>
+  </si>
+  <si>
+    <t>RIB7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00124</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pyridoxal-P biosynthesis, erythrose-4P =&gt; pyridoxal-P</t>
+  </si>
+  <si>
+    <t>pdxB, pdxA, pdxJ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00115</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAD biosynthesis, aspartate =&gt; quinolinate =&gt; NAD</t>
+  </si>
+  <si>
+    <t>nadB, nadX, nadA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00119</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pantothenate biosynthesis, valine/L-aspartate =&gt; pantothenate</t>
+  </si>
+  <si>
+    <t>panD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>panD, panC-cmk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00913</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pantothenate biosynthesis, 2-oxoisovalerate/spermine =&gt; pantothenate</t>
+  </si>
+  <si>
+    <t>panC-cmk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00120</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coenzyme A biosynthesis, pantothenate =&gt; CoA</t>
+  </si>
+  <si>
+    <t>PPCDC, E2.7.7.3B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00914</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coenzyme A biosynthesis, archaea, 2-oxoisovalerate =&gt; 4-phosphopantoate =&gt; CoA</t>
+  </si>
+  <si>
+    <t>M00572</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pimeloyl-ACP biosynthesis, BioC-BioH pathway, malonyl-ACP =&gt; pimeloyl-ACP</t>
+  </si>
+  <si>
+    <t>M00123</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biotin biosynthesis, pimeloyl-ACP/CoA =&gt; biotin</t>
+  </si>
+  <si>
+    <t>bioB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bioF, bioB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00950</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biotin biosynthesis, BioU pathway, pimeloyl-ACP/CoA =&gt; biotin</t>
+  </si>
+  <si>
+    <t>M00573</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biotin biosynthesis, BioI pathway, long-chain-acyl-ACP =&gt; pimeloyl-ACP =&gt; biotin</t>
+  </si>
+  <si>
+    <t>M00577</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biotin biosynthesis, BioW pathway, pimelate =&gt; pimeloyl-CoA =&gt; biotin</t>
+  </si>
+  <si>
+    <t>M00883</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lipoic acid biosynthesis, animals and bacteria, octanoyl-ACP =&gt; dihydrolipoyl-H =&gt; dihydrolipoyl-E2</t>
+  </si>
+  <si>
+    <t>lipL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00126</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tetrahydrofolate biosynthesis, GTP =&gt; THF</t>
+  </si>
+  <si>
+    <t>nudB, E3.5.4.16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00840</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tetrahydrofolate biosynthesis, mediated by ribA and trpF, GTP =&gt; THF</t>
+  </si>
+  <si>
+    <t>folKP, folC2, DHFR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00841</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tetrahydrofolate biosynthesis, mediated by PTPS, GTP =&gt; THF</t>
+  </si>
+  <si>
+    <t>M00843</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L-threo-Tetrahydrobiopterin biosynthesis, GTP =&gt; L-threo-BH4</t>
+  </si>
+  <si>
+    <t>M00880</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molybdenum cofactor biosynthesis, GTP =&gt; molybdenum cofactor</t>
+  </si>
+  <si>
+    <t>M00140</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1-unit interconversion, prokaryotes</t>
+  </si>
+  <si>
+    <t>M00846</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siroheme biosynthesis, glutamyl-tRNA =&gt; siroheme</t>
+  </si>
+  <si>
+    <t>hemX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00868</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heme biosynthesis, animals and fungi, glycine =&gt; heme</t>
+  </si>
+  <si>
+    <t>hemE, hemN, hemG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00121</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heme biosynthesis, plants and bacteria, glutamate =&gt; heme</t>
+  </si>
+  <si>
+    <t>M00926</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heme biosynthesis, bacteria, glutamyl-tRNA =&gt; coproporphyrin III =&gt; heme</t>
+  </si>
+  <si>
+    <t>M00847</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heme biosynthesis, archaea, siroheme =&gt; heme</t>
+  </si>
+  <si>
+    <t>ahbAB, ahbC, ahbD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00924</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cobalamin biosynthesis, anaerobic, uroporphyrinogen III =&gt; sirohydrochlorin =&gt; cobyrinate a,c-diamide</t>
+  </si>
+  <si>
+    <t>M00925</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cobalamin biosynthesis, aerobic, uroporphyrinogen III =&gt; precorrin 2 =&gt; cobyrinate a,c-diamide</t>
+  </si>
+  <si>
+    <t>M00122</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cobalamin biosynthesis, cobyrinate a,c-diamide =&gt; cobalamin</t>
+  </si>
+  <si>
+    <t>M00836</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coenzyme F430 biosynthesis, sirohydrochlorin =&gt; coenzyme F430</t>
+  </si>
+  <si>
+    <t>cfbA, cfbB, cfbC, cfbD, cfbE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00117</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubiquinone biosynthesis, prokaryotes, chorismate (+ polyprenyl-PP) =&gt; ubiquinol</t>
+  </si>
+  <si>
+    <t>xanB2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00116</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menaquinone biosynthesis, chorismate (+ polyprenyl-PP) =&gt; menaquinol</t>
+  </si>
+  <si>
+    <t>menA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E3.1.2.28</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00930</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menaquinone biosynthesis, futalosine pathway</t>
+  </si>
+  <si>
+    <t>mqnX, mqnB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00932</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phylloquinone biosynthesis, chorismate (+ phytyl-PP) =&gt; phylloquinol</t>
+  </si>
+  <si>
+    <t>M00112</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tocopherol/tocotorienol biosynthesis, homogentisate + phytyl/geranylgeranyl-PP =&gt; tocopherol/tocotorienol</t>
+  </si>
+  <si>
+    <t>HPT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00933</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plastoquinone biosynthesis, homogentisate + solanesyl-PP =&gt; plastoquinol</t>
+  </si>
+  <si>
+    <t>HST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00002</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycolysis, core module involving three-carbon compounds</t>
+  </si>
+  <si>
+    <t>gapor, gap2, apgM, PK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Citrate cycle, first carbon oxidation, oxaloacetate =&gt; 2-oxoglutarate</t>
+  </si>
+  <si>
+    <t>acnB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pentose phosphate pathway, non-oxidative phase, fructose 6P =&gt; ribose 5P</t>
+  </si>
+  <si>
+    <t>M00580</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pentose phosphate pathway, archaea, fructose 6P =&gt; ribose 5P</t>
+  </si>
+  <si>
+    <t>fae-hps, hps-phi, pfkA, pfkB, FBA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hxlB, fae-hps, hps-phi, pfkA, FBA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thrH, psp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thrH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00018</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Threonine biosynthesis, aspartate =&gt; homoserine =&gt; threonine</t>
+  </si>
+  <si>
+    <t>M00021</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cysteine biosynthesis, serine =&gt; cysteine</t>
+  </si>
+  <si>
+    <t>cysE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00609</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cysteine biosynthesis, methionine =&gt; cysteine</t>
+  </si>
+  <si>
+    <t>yrrT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mccA, yrrT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00017</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methionine biosynthesis, aspartate =&gt; homoserine =&gt; methionine</t>
+  </si>
+  <si>
+    <t>hom, thrA, metL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00019</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valine/isoleucine biosynthesis, pyruvate =&gt; valine / 2-oxobutanoate =&gt; isoleucine</t>
+  </si>
+  <si>
+    <t>E2.2.1.6S</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00535</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Isoleucine biosynthesis, pyruvate =&gt; 2-oxobutanoate</t>
+  </si>
+  <si>
+    <t>cimA, leuC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00570</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Isoleucine biosynthesis, threonine =&gt; 2-oxobutanoate =&gt; isoleucine</t>
+  </si>
+  <si>
+    <t>M00432</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leucine biosynthesis, 2-oxoisovalerate =&gt; 2-oxoisocaproate</t>
+  </si>
+  <si>
+    <t>leuA, leuC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00016</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, succinyl-DAP pathway, aspartate =&gt; lysine</t>
+  </si>
+  <si>
+    <t>dapB, dapF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thrA, metL, lysA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00525</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, acetyl-DAP pathway, aspartate =&gt; lysine</t>
+  </si>
+  <si>
+    <t>M00526</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, DAP dehydrogenase pathway, aspartate =&gt; lysine</t>
+  </si>
+  <si>
+    <t>dapB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thrA, metL, dapdh, lysA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00527</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, DAP aminotransferase pathway, aspartate =&gt; lysine</t>
+  </si>
+  <si>
+    <t>thrA, metL, E2.6.1.83, lysA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00030</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, AAA pathway, 2-oxoglutarate =&gt; 2-aminoadipate =&gt; lysine</t>
+  </si>
+  <si>
+    <t>LYS4, LYS12, LYS9, LYS1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00433</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, 2-oxoglutarate =&gt; 2-oxoadipate</t>
+  </si>
+  <si>
+    <t>LYS4, aksD, aksE, LYS12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00031</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine biosynthesis, mediated by LysW, 2-aminoadipate =&gt; lysine</t>
+  </si>
+  <si>
+    <t>lysX, lysY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lysX, lysY, lysJ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00028</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ornithine biosynthesis, glutamate =&gt; ornithine</t>
+  </si>
+  <si>
+    <t>M00763</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ornithine biosynthesis, mediated by LysW, glutamate =&gt; ornithine</t>
+  </si>
+  <si>
+    <t>lysY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lysY, lysJ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00844</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arginine biosynthesis, ornithine =&gt; arginine</t>
+  </si>
+  <si>
+    <t>argHA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00845</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arginine biosynthesis, glutamate =&gt; acetylcitrulline =&gt; arginine</t>
+  </si>
+  <si>
+    <t>argF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00029</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Urea cycle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00026</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Histidine biosynthesis, PRPP =&gt; histidine</t>
+  </si>
+  <si>
+    <t>hisG, hisE, hisA, hisH, hisB, hisD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shikimate pathway, phosphoenolpyruvate + erythrose-4P =&gt; chorismate</t>
+  </si>
+  <si>
+    <t>M00023</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tryptophan biosynthesis, chorismate =&gt; tryptophan</t>
+  </si>
+  <si>
+    <t>trpB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>trpGD, trpB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00024</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phenylalanine biosynthesis, chorismate =&gt; phenylpyruvate =&gt; phenylalanine</t>
+  </si>
+  <si>
+    <t>E5.4.99.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M00910</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phenylalanine biosynthesis, chorismate =&gt; arogenate =&gt; phenylalanine</t>
+  </si>
+  <si>
+    <t>M00025</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tyrosine biosynthesis, chorismate =&gt; HPP =&gt; tyrosine</t>
+  </si>
+  <si>
+    <t>M00040</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tyrosine biosynthesis, chorismate =&gt; arogenate =&gt; tyrosine</t>
+  </si>
+  <si>
+    <t>E5.4.99.5, pheA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fwdA, fwdB, fwdC, fwdD, fwdE, fwdF, fwdG, fwdH, ftr, mch, mtd, mtrA, mtrC, mtrD, mtrE, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fwdA, fwdB, fwdC, fwdD, fwdF, fwdG, fwdH, ftr, mch, mtd, mtrA, mtrB, mtrC, mtrD, mtrE, mtrF, mtrG, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pta, cdhC, cdhE, cdhD, mtrA, mtrB, mtrC, mtrD, mtrE, mtrF, mtrG, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtmB, mtbC, mtbB, mttC, mttB, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtbA, mtmB, mtbC, mtbB, mttC, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmoX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ackA, pta, cdhC, cdhE, cdhD, mtrA, mtrC, mtrD, mtrE, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtaA, mtaB, mtaC, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmoA-amoA, pmoB-amoB, pmoC-amoC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>glyA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fae-hps, hxlB, hps-phi, pfkA, pfkB, FBA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FBA, FBP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cofG, cofH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mfnB, mfnE, mfnA, mfnD, mfnF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mfnB, mfnC, mfnE, mfnD, mfnF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cdhA, cdhB, cdhC, cdhE, cdhD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AK9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAD, pyrB, pyrI, pyrD, DHODH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAD, URA2, pyrI, pyrBI, pyrD, DHODH, UMPS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thiF, thiH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thiN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ribB, FHY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RIB7, ribB, FLAD1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>coaA, coaB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pok, pps, dpck</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pok, pps, dpck, E2.7.7.3B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fabB, fabF, bioG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fabB, bioG, bioK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E3.5.4.16, E3.1.3.1, folKP, DHFR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>folKP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spr1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOCS1, mogA, moaB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOCS1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hemE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cfbA, cbiG, cbiT, cbiE, cobH-cbiC,  cobB-cbiA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cbiK, cfbA, cbiG, cbiT, cbiE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cobH-cbiC, cobB-cbiA, cobS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MMAB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mqnX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gapor, gap2, apgM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E2.2.1.1, rpiB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rpiB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hxlB, hps-phi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hps-phi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hom, thrA, metL, thrH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>leuC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dapH, lysA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dapB, E2.6.1.83, dapF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LYS4, LYS9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LYS4, aksD, aksE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>argHA, argO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hisI, hisA, hisH, hisF, hisB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aroQ, aroE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> aroG, aroD, aroE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tyrA, AROA1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E5.4.99.5, tyrA, AROA1, pheA, pheC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AROA1, tyrA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E5.4.99.5, pheA, AROA1, tyrA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tyrC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pathway Module</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Methanogenesis, CO2 =&gt; methane</t>
-  </si>
-  <si>
-    <t>M00357</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methanogenesis, acetate =&gt; methane</t>
-  </si>
-  <si>
-    <t>M00356</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methanogenesis, methanol =&gt; methane</t>
-  </si>
-  <si>
-    <t>M00563</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methanogenesis, methylamine/dimethylamine/trimethylamine =&gt; methane</t>
-  </si>
-  <si>
-    <t>M00358</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coenzyme M biosynthesis</t>
-  </si>
-  <si>
-    <t>M00608</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-Oxocarboxylic acid chain extension, 2-oxoglutarate =&gt; 2-oxoadipate =&gt; 2-oxopimelate =&gt; 2-oxosuberate</t>
-  </si>
-  <si>
-    <t>M00174</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methane oxidation, methanotroph, methane =&gt; formaldehyde</t>
-  </si>
-  <si>
-    <t>M00346</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Formaldehyde assimilation, serine pathway</t>
-  </si>
-  <si>
-    <t>M00345</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Formaldehyde assimilation, ribulose monophosphate pathway</t>
-  </si>
-  <si>
-    <t>M00344</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Formaldehyde assimilation, xylulose monophosphate pathway</t>
-  </si>
-  <si>
-    <t>M00378</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>F420 biosynthesis, archaea</t>
-  </si>
-  <si>
-    <t>M00935</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methanofuran biosynthesis</t>
-  </si>
-  <si>
-    <t>M00422</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Acetyl-CoA pathway, CO2 =&gt; acetyl-CoA</t>
-  </si>
-  <si>
-    <t>M00020</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Serine biosynthesis, glycerate-3P =&gt; serine</t>
-  </si>
-  <si>
-    <t>M00129</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ascorbate biosynthesis, animals, glucose-1P =&gt; ascorbate</t>
-  </si>
-  <si>
-    <t>uidA, AKR1A1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00114</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ascorbate biosynthesis, plants, fructose-6P =&gt; ascorbate</t>
-  </si>
-  <si>
-    <t>GMPP, VTC4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>comB, comC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>comA, comB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>aksA, aksD, aksE, aksF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cofH, cofG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mfnA, mfnD, mfnF, mfnE, mfnB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mfnD, mfnF, mfnE, mfnC, mfnB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00049</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adenine ribonucleotide biosynthesis, IMP =&gt; ADP,ATP</t>
-  </si>
-  <si>
-    <t>M00051</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>De novo pyrimidine biosynthesis, glutamine (+ PRPP) =&gt; UMP</t>
-  </si>
-  <si>
-    <t>M00127</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thiamine biosynthesis, prokaryotes, AIR (+ DXP/tyrosine) =&gt; TMP/TPP</t>
-  </si>
-  <si>
-    <t>M00896</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thiamine biosynthesis, archaea, AIR (+ NAD+) =&gt; TMP/TPP</t>
-  </si>
-  <si>
-    <t>M00125</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Riboflavin biosynthesis, plants and bacteria, GTP =&gt; riboflavin/FMN/FAD</t>
-  </si>
-  <si>
-    <t>ribD1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00911</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Riboflavin biosynthesis, fungi, GTP =&gt; riboflavin/FMN/FAD</t>
-  </si>
-  <si>
-    <t>RIB7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00124</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pyridoxal-P biosynthesis, erythrose-4P =&gt; pyridoxal-P</t>
-  </si>
-  <si>
-    <t>pdxB, pdxA, pdxJ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NAD biosynthesis, aspartate =&gt; quinolinate =&gt; NAD</t>
-  </si>
-  <si>
-    <t>nadB, nadX, nadA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00119</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pantothenate biosynthesis, valine/L-aspartate =&gt; pantothenate</t>
-  </si>
-  <si>
-    <t>panD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>panD, panC-cmk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00913</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pantothenate biosynthesis, 2-oxoisovalerate/spermine =&gt; pantothenate</t>
-  </si>
-  <si>
-    <t>panC-cmk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00120</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coenzyme A biosynthesis, pantothenate =&gt; CoA</t>
-  </si>
-  <si>
-    <t>PPCDC, E2.7.7.3B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00914</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coenzyme A biosynthesis, archaea, 2-oxoisovalerate =&gt; 4-phosphopantoate =&gt; CoA</t>
-  </si>
-  <si>
-    <t>M00572</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pimeloyl-ACP biosynthesis, BioC-BioH pathway, malonyl-ACP =&gt; pimeloyl-ACP</t>
-  </si>
-  <si>
-    <t>M00123</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biotin biosynthesis, pimeloyl-ACP/CoA =&gt; biotin</t>
-  </si>
-  <si>
-    <t>bioB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bioF, bioB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00950</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biotin biosynthesis, BioU pathway, pimeloyl-ACP/CoA =&gt; biotin</t>
-  </si>
-  <si>
-    <t>M00573</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biotin biosynthesis, BioI pathway, long-chain-acyl-ACP =&gt; pimeloyl-ACP =&gt; biotin</t>
-  </si>
-  <si>
-    <t>M00577</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biotin biosynthesis, BioW pathway, pimelate =&gt; pimeloyl-CoA =&gt; biotin</t>
-  </si>
-  <si>
-    <t>M00883</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lipoic acid biosynthesis, animals and bacteria, octanoyl-ACP =&gt; dihydrolipoyl-H =&gt; dihydrolipoyl-E2</t>
-  </si>
-  <si>
-    <t>lipL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00126</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tetrahydrofolate biosynthesis, GTP =&gt; THF</t>
-  </si>
-  <si>
-    <t>nudB, E3.5.4.16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00840</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tetrahydrofolate biosynthesis, mediated by ribA and trpF, GTP =&gt; THF</t>
-  </si>
-  <si>
-    <t>folKP, folC2, DHFR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00841</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tetrahydrofolate biosynthesis, mediated by PTPS, GTP =&gt; THF</t>
-  </si>
-  <si>
-    <t>M00843</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>L-threo-Tetrahydrobiopterin biosynthesis, GTP =&gt; L-threo-BH4</t>
-  </si>
-  <si>
-    <t>M00880</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Molybdenum cofactor biosynthesis, GTP =&gt; molybdenum cofactor</t>
-  </si>
-  <si>
-    <t>M00140</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C1-unit interconversion, prokaryotes</t>
-  </si>
-  <si>
-    <t>M00846</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Siroheme biosynthesis, glutamyl-tRNA =&gt; siroheme</t>
-  </si>
-  <si>
-    <t>hemX</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00868</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heme biosynthesis, animals and fungi, glycine =&gt; heme</t>
-  </si>
-  <si>
-    <t>hemE, hemN, hemG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00121</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heme biosynthesis, plants and bacteria, glutamate =&gt; heme</t>
-  </si>
-  <si>
-    <t>M00926</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heme biosynthesis, bacteria, glutamyl-tRNA =&gt; coproporphyrin III =&gt; heme</t>
-  </si>
-  <si>
-    <t>M00847</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heme biosynthesis, archaea, siroheme =&gt; heme</t>
-  </si>
-  <si>
-    <t>ahbAB, ahbC, ahbD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00924</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cobalamin biosynthesis, anaerobic, uroporphyrinogen III =&gt; sirohydrochlorin =&gt; cobyrinate a,c-diamide</t>
-  </si>
-  <si>
-    <t>M00925</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cobalamin biosynthesis, aerobic, uroporphyrinogen III =&gt; precorrin 2 =&gt; cobyrinate a,c-diamide</t>
-  </si>
-  <si>
-    <t>M00122</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cobalamin biosynthesis, cobyrinate a,c-diamide =&gt; cobalamin</t>
-  </si>
-  <si>
-    <t>M00836</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coenzyme F430 biosynthesis, sirohydrochlorin =&gt; coenzyme F430</t>
-  </si>
-  <si>
-    <t>cfbA, cfbB, cfbC, cfbD, cfbE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00117</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ubiquinone biosynthesis, prokaryotes, chorismate (+ polyprenyl-PP) =&gt; ubiquinol</t>
-  </si>
-  <si>
-    <t>xanB2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00116</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Menaquinone biosynthesis, chorismate (+ polyprenyl-PP) =&gt; menaquinol</t>
-  </si>
-  <si>
-    <t>menA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E3.1.2.28</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00930</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Menaquinone biosynthesis, futalosine pathway</t>
-  </si>
-  <si>
-    <t>mqnX, mqnB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00932</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phylloquinone biosynthesis, chorismate (+ phytyl-PP) =&gt; phylloquinol</t>
-  </si>
-  <si>
-    <t>M00112</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tocopherol/tocotorienol biosynthesis, homogentisate + phytyl/geranylgeranyl-PP =&gt; tocopherol/tocotorienol</t>
-  </si>
-  <si>
-    <t>HPT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00933</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plastoquinone biosynthesis, homogentisate + solanesyl-PP =&gt; plastoquinol</t>
-  </si>
-  <si>
-    <t>HST</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00002</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Glycolysis, core module involving three-carbon compounds</t>
-  </si>
-  <si>
-    <t>gapor, gap2, apgM, PK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00010</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Citrate cycle, first carbon oxidation, oxaloacetate =&gt; 2-oxoglutarate</t>
-  </si>
-  <si>
-    <t>acnB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pentose phosphate pathway, non-oxidative phase, fructose 6P =&gt; ribose 5P</t>
-  </si>
-  <si>
-    <t>M00580</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pentose phosphate pathway, archaea, fructose 6P =&gt; ribose 5P</t>
-  </si>
-  <si>
-    <t>fae-hps, hps-phi, pfkA, pfkB, FBA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hxlB, fae-hps, hps-phi, pfkA, FBA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>thrH, psp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>thrH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00018</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Threonine biosynthesis, aspartate =&gt; homoserine =&gt; threonine</t>
-  </si>
-  <si>
-    <t>M00021</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cysteine biosynthesis, serine =&gt; cysteine</t>
-  </si>
-  <si>
-    <t>cysE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00609</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cysteine biosynthesis, methionine =&gt; cysteine</t>
-  </si>
-  <si>
-    <t>yrrT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mccA, yrrT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00017</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methionine biosynthesis, aspartate =&gt; homoserine =&gt; methionine</t>
-  </si>
-  <si>
-    <t>hom, thrA, metL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00019</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valine/isoleucine biosynthesis, pyruvate =&gt; valine / 2-oxobutanoate =&gt; isoleucine</t>
-  </si>
-  <si>
-    <t>E2.2.1.6S</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00535</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Isoleucine biosynthesis, pyruvate =&gt; 2-oxobutanoate</t>
-  </si>
-  <si>
-    <t>cimA, leuC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00570</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Isoleucine biosynthesis, threonine =&gt; 2-oxobutanoate =&gt; isoleucine</t>
-  </si>
-  <si>
-    <t>M00432</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leucine biosynthesis, 2-oxoisovalerate =&gt; 2-oxoisocaproate</t>
-  </si>
-  <si>
-    <t>leuA, leuC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00016</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, succinyl-DAP pathway, aspartate =&gt; lysine</t>
-  </si>
-  <si>
-    <t>dapB, dapF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>thrA, metL, lysA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00525</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, acetyl-DAP pathway, aspartate =&gt; lysine</t>
-  </si>
-  <si>
-    <t>M00526</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, DAP dehydrogenase pathway, aspartate =&gt; lysine</t>
-  </si>
-  <si>
-    <t>dapB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>thrA, metL, dapdh, lysA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00527</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, DAP aminotransferase pathway, aspartate =&gt; lysine</t>
-  </si>
-  <si>
-    <t>thrA, metL, E2.6.1.83, lysA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00030</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, AAA pathway, 2-oxoglutarate =&gt; 2-aminoadipate =&gt; lysine</t>
-  </si>
-  <si>
-    <t>LYS4, LYS12, LYS9, LYS1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00433</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, 2-oxoglutarate =&gt; 2-oxoadipate</t>
-  </si>
-  <si>
-    <t>LYS4, aksD, aksE, LYS12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00031</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lysine biosynthesis, mediated by LysW, 2-aminoadipate =&gt; lysine</t>
-  </si>
-  <si>
-    <t>lysX, lysY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lysX, lysY, lysJ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00028</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ornithine biosynthesis, glutamate =&gt; ornithine</t>
-  </si>
-  <si>
-    <t>M00763</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ornithine biosynthesis, mediated by LysW, glutamate =&gt; ornithine</t>
-  </si>
-  <si>
-    <t>lysY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lysY, lysJ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00844</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Arginine biosynthesis, ornithine =&gt; arginine</t>
-  </si>
-  <si>
-    <t>argHA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00845</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Arginine biosynthesis, glutamate =&gt; acetylcitrulline =&gt; arginine</t>
-  </si>
-  <si>
-    <t>argF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00029</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Urea cycle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00026</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Histidine biosynthesis, PRPP =&gt; histidine</t>
-  </si>
-  <si>
-    <t>hisG, hisE, hisA, hisH, hisB, hisD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00022</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shikimate pathway, phosphoenolpyruvate + erythrose-4P =&gt; chorismate</t>
-  </si>
-  <si>
-    <t>M00023</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tryptophan biosynthesis, chorismate =&gt; tryptophan</t>
-  </si>
-  <si>
-    <t>trpB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>trpGD, trpB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00024</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phenylalanine biosynthesis, chorismate =&gt; phenylpyruvate =&gt; phenylalanine</t>
-  </si>
-  <si>
-    <t>E5.4.99.5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>M00910</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phenylalanine biosynthesis, chorismate =&gt; arogenate =&gt; phenylalanine</t>
-  </si>
-  <si>
-    <t>M00025</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tyrosine biosynthesis, chorismate =&gt; HPP =&gt; tyrosine</t>
-  </si>
-  <si>
-    <t>M00040</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tyrosine biosynthesis, chorismate =&gt; arogenate =&gt; tyrosine</t>
-  </si>
-  <si>
-    <t>E5.4.99.5, pheA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fwdA, fwdB, fwdC, fwdD, fwdE, fwdF, fwdG, fwdH, ftr, mch, mtd, mtrA, mtrC, mtrD, mtrE, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fwdA, fwdB, fwdC, fwdD, fwdF, fwdG, fwdH, ftr, mch, mtd, mtrA, mtrB, mtrC, mtrD, mtrE, mtrF, mtrG, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pta, cdhC, cdhE, cdhD, mtrA, mtrB, mtrC, mtrD, mtrE, mtrF, mtrG, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mtmB, mtbC, mtbB, mttC, mttB, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mtbA, mtmB, mtbC, mtbB, mttC, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mmoX</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ackA, pta, cdhC, cdhE, cdhD, mtrA, mtrC, mtrD, mtrE, mtrH, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mtaA, mtaB, mtaC, mcrA, mcrB, mcrG, hdrA1, hdrB1, hdrC1, hdrA2, hdrB2, hdrC2, hdrD, hdrE, mvhD, mvhA, mvhG, fdhB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pmoA-amoA, pmoB-amoB, pmoC-amoC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>glyA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fae-hps, hxlB, hps-phi, pfkA, pfkB, FBA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FBA, FBP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cofG, cofH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mfnB, mfnE, mfnA, mfnD, mfnF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mfnB, mfnC, mfnE, mfnD, mfnF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cdhA, cdhB, cdhC, cdhE, cdhD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AK9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CAD, pyrB, pyrI, pyrD, DHODH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CAD, URA2, pyrI, pyrBI, pyrD, DHODH, UMPS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>thiF, thiH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>thiN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ribB, FHY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RIB7, ribB, FLAD1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>coaA, coaB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pok, pps, dpck</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pok, pps, dpck, E2.7.7.3B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fabB, fabF, bioG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fabB, bioG, bioK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E3.5.4.16, E3.1.3.1, folKP, DHFR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>folKP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>spr1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOCS1, mogA, moaB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOCS1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hemE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cfbA, cbiG, cbiT, cbiE, cobH-cbiC,  cobB-cbiA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cbiK, cfbA, cbiG, cbiT, cbiE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cobH-cbiC, cobB-cbiA, cobS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MMAB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mqnX</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gapor, gap2, apgM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E2.2.1.1, rpiB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>rpiB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hxlB, hps-phi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hps-phi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hom, thrA, metL, thrH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>leuC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>dapH, lysA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>dapB, E2.6.1.83, dapF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LYS4, LYS9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LYS4, aksD, aksE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>argHA, argO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hisI, hisA, hisH, hisF, hisB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>aroQ, aroE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> aroG, aroD, aroE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tyrA, AROA1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E5.4.99.5, tyrA, AROA1, pheA, pheC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AROA1, tyrA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E5.4.99.5, pheA, AROA1, tyrA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tyrC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pathway Module</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2216,7 +2217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2225,6 +2226,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2514,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2714,25 +2718,25 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="56" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>6</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>0</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2806,25 +2810,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="42" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="3">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3151,48 +3155,48 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="98" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="3">
         <v>15</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="3">
         <v>7</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="F28" s="3">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="42" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="3">
         <v>4</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="3">
         <v>0</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="3">
         <v>3</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3342,7 +3346,7 @@
         <v>8</v>
       </c>
       <c r="D36" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>128</v>
@@ -3493,25 +3497,25 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="42" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="4">
         <v>3</v>
       </c>
-      <c r="D43" s="1">
-        <v>2</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="D43" s="4">
+        <v>2</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F43" s="1">
-        <v>2</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="F43" s="4">
+        <v>2</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3838,25 +3842,25 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="56" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>5</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>4</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F58" s="2">
-        <v>2</v>
-      </c>
-      <c r="G58" s="2" t="s">
+      <c r="F58" s="1">
+        <v>2</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4009,8 +4013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC54B323-3F56-40F5-B77E-A33C52802FB6}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4029,7 +4033,7 @@
         <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>90</v>
@@ -4052,7 +4056,7 @@
         <v>205</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>206</v>
+        <v>498</v>
       </c>
       <c r="C2" s="1">
         <v>37</v>
@@ -4061,21 +4065,21 @@
         <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F2" s="1">
         <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="C3" s="1">
         <v>30</v>
@@ -4084,21 +4088,21 @@
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F3" s="1">
         <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C4" s="1">
         <v>19</v>
@@ -4107,21 +4111,21 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F4" s="1">
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="C5" s="1">
         <v>23</v>
@@ -4130,21 +4134,21 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F5" s="1">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -4153,21 +4157,21 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -4176,21 +4180,21 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="C8" s="1">
         <v>12</v>
@@ -4199,21 +4203,21 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -4228,15 +4232,15 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
@@ -4245,21 +4249,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F10" s="1">
         <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -4268,21 +4272,21 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -4291,21 +4295,21 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
@@ -4314,21 +4318,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F13" s="1">
         <v>5</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -4337,21 +4341,21 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F14" s="1">
         <v>5</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
@@ -4360,13 +4364,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F15" s="1">
         <v>2</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -4380,7 +4384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8004DF0-0861-46FF-AE46-C3D55CE235CC}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -4421,10 +4425,10 @@
     </row>
     <row r="2" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="C2" s="1">
         <v>7</v>
@@ -4439,15 +4443,15 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
@@ -4462,15 +4466,15 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
@@ -4479,21 +4483,21 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -4502,21 +4506,21 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F5" s="1">
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -4525,21 +4529,21 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -4548,21 +4552,21 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F7" s="1">
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -4577,15 +4581,15 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="C9" s="1">
         <v>15</v>
@@ -4594,21 +4598,21 @@
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F9" s="1">
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="C10" s="1">
         <v>11</v>
@@ -4617,21 +4621,21 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
@@ -4640,21 +4644,21 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="C12" s="1">
         <v>17</v>
@@ -4663,21 +4667,21 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="C13" s="1">
         <v>8</v>
@@ -4686,21 +4690,21 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F13" s="1">
         <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="C14" s="1">
         <v>6</v>
@@ -4709,21 +4713,21 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="C15" s="1">
         <v>8</v>
@@ -4732,21 +4736,21 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
@@ -4755,21 +4759,21 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -4784,15 +4788,15 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="C18" s="1">
         <v>12</v>
@@ -4801,21 +4805,21 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F18" s="1">
         <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="C19" s="1">
         <v>7</v>
@@ -4824,21 +4828,21 @@
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F19" s="1">
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="C20" s="1">
         <v>10</v>
@@ -4847,21 +4851,21 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F20" s="1">
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="C21" s="1">
         <v>6</v>
@@ -4870,21 +4874,21 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
@@ -4893,21 +4897,21 @@
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -4916,21 +4920,21 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
@@ -4939,21 +4943,21 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -4962,21 +4966,21 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="C26" s="1">
         <v>17</v>
@@ -4985,21 +4989,21 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F26" s="1">
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="C27" s="1">
         <v>6</v>
@@ -5014,15 +5018,15 @@
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="C28" s="1">
         <v>5</v>
@@ -5037,15 +5041,15 @@
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
@@ -5060,15 +5064,15 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="C30" s="1">
         <v>9</v>
@@ -5077,21 +5081,21 @@
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="C31" s="1">
         <v>5</v>
@@ -5106,15 +5110,15 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="C32" s="1">
         <v>14</v>
@@ -5123,21 +5127,21 @@
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="C33" s="1">
         <v>8</v>
@@ -5146,21 +5150,21 @@
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="C34" s="1">
         <v>15</v>
@@ -5169,21 +5173,21 @@
         <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F34" s="1">
         <v>3</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="C35" s="1">
         <v>10</v>
@@ -5192,21 +5196,21 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="C36" s="1">
         <v>4</v>
@@ -5215,21 +5219,21 @@
         <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F36" s="1">
         <v>3</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="C37" s="1">
         <v>21</v>
@@ -5238,21 +5242,21 @@
         <v>6</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F37" s="1">
         <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="C38" s="1">
         <v>16</v>
@@ -5261,7 +5265,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -5272,10 +5276,10 @@
     </row>
     <row r="39" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="C39" s="1">
         <v>10</v>
@@ -5284,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -5295,10 +5299,10 @@
     </row>
     <row r="40" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="C40" s="1">
         <v>5</v>
@@ -5307,21 +5311,21 @@
         <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F40" s="1">
         <v>5</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="C41" s="1">
         <v>11</v>
@@ -5330,7 +5334,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -5341,10 +5345,10 @@
     </row>
     <row r="42" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="C42" s="1">
         <v>9</v>
@@ -5353,7 +5357,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -5364,10 +5368,10 @@
     </row>
     <row r="43" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="C43" s="1">
         <v>7</v>
@@ -5376,21 +5380,21 @@
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F43" s="1">
         <v>2</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="C44" s="1">
         <v>13</v>
@@ -5405,15 +5409,15 @@
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>341</v>
       </c>
       <c r="C45" s="1">
         <v>5</v>
@@ -5428,15 +5432,15 @@
         <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
@@ -5451,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -5506,10 +5510,10 @@
     </row>
     <row r="2" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="C2" s="1">
         <v>12</v>
@@ -5518,21 +5522,21 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="C3" s="1">
         <v>6</v>
@@ -5541,21 +5545,21 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
@@ -5564,21 +5568,21 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
@@ -5587,21 +5591,21 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -5610,21 +5614,21 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F6" s="1">
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C7" s="1">
         <v>7</v>
@@ -5633,21 +5637,21 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F7" s="1">
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
@@ -5656,21 +5660,21 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -5679,21 +5683,21 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -5702,21 +5706,21 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="C11" s="1">
         <v>6</v>
@@ -5725,21 +5729,21 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="C12" s="1">
         <v>13</v>
@@ -5754,15 +5758,15 @@
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
@@ -5771,7 +5775,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -5782,10 +5786,10 @@
     </row>
     <row r="14" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -5794,21 +5798,21 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="C15" s="1">
         <v>8</v>
@@ -5817,7 +5821,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -5828,10 +5832,10 @@
     </row>
     <row r="16" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -5840,21 +5844,21 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="C17" s="1">
         <v>13</v>
@@ -5863,21 +5867,21 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F17" s="1">
         <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="C18" s="1">
         <v>9</v>
@@ -5886,21 +5890,21 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F18" s="1">
         <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="C19" s="1">
         <v>9</v>
@@ -5909,21 +5913,21 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F19" s="1">
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>394</v>
       </c>
       <c r="C20" s="1">
         <v>10</v>
@@ -5932,21 +5936,21 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F20" s="1">
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="C21" s="1">
         <v>9</v>
@@ -5955,21 +5959,21 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>400</v>
       </c>
       <c r="C22" s="1">
         <v>6</v>
@@ -5978,21 +5982,21 @@
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F22" s="1">
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>403</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
@@ -6001,21 +6005,21 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F23" s="1">
         <v>3</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="C24" s="1">
         <v>16</v>
@@ -6030,15 +6034,15 @@
         <v>2</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
@@ -6047,21 +6051,21 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>413</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -6076,15 +6080,15 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="C27" s="1">
         <v>7</v>
@@ -6093,21 +6097,21 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="C28" s="1">
         <v>6</v>
@@ -6122,15 +6126,15 @@
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="C29" s="1">
         <v>19</v>
@@ -6139,21 +6143,21 @@
         <v>6</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F29" s="1">
         <v>5</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>424</v>
       </c>
       <c r="C30" s="1">
         <v>14</v>
@@ -6162,21 +6166,21 @@
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="C31" s="1">
         <v>15</v>
@@ -6185,21 +6189,21 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="C32" s="1">
         <v>13</v>
@@ -6208,21 +6212,21 @@
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F32" s="1">
         <v>5</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>433</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
@@ -6237,15 +6241,15 @@
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>435</v>
       </c>
       <c r="C34" s="1">
         <v>12</v>
@@ -6254,21 +6258,21 @@
         <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F34" s="1">
         <v>4</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>437</v>
       </c>
       <c r="C35" s="1">
         <v>8</v>
@@ -6277,13 +6281,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F35" s="1">
         <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>